<commit_message>
Feat: comment & reply order 기준 정할 수 있도록 수
</commit_message>
<xml_diff>
--- a/youtube/input.xlsx
+++ b/youtube/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agayo\Desktop\크몽\kmong_crawler\youtube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD326DB9-C8A1-4C7E-8B25-24D56EB14DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB40F9E-88A3-4231-9801-2D8EA0550A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{18DD557C-6457-4FB1-94E7-5CF6DC40C30F}"/>
+    <workbookView xWindow="8460" yWindow="2025" windowWidth="28800" windowHeight="12450" xr2:uid="{18DD557C-6457-4FB1-94E7-5CF6DC40C30F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,17 +35,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>https://www.youtube.com/watch?v=0UKwpJUUDlM</t>
+    <t>https://www.youtube.com/shorts/xspWfbOSsms</t>
   </si>
   <si>
-    <t>https://www.youtube.com/shorts/qmQ_lzNtQco</t>
+    <t>https://www.youtube.com/watch?v=eb6cJMSZuWo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +57,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -79,18 +89,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,12 +433,15 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6FBC8090-0255-4247-8143-0F29E409358F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>